<commit_message>
disaster and other changes:
</commit_message>
<xml_diff>
--- a/data/output_data3.xlsx
+++ b/data/output_data3.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">Turn #1: Foremz: </t>
   </si>
   <si>
-    <t xml:space="preserve">Turn #1: hello: </t>
+    <t xml:space="preserve">Turn #1: Hello: </t>
   </si>
   <si>
     <t xml:space="preserve">Turn #2: Brobdingnag: </t>
@@ -40,7 +40,7 @@
     <t xml:space="preserve">Turn #2: Foremz: </t>
   </si>
   <si>
-    <t xml:space="preserve">Turn #2: hello: </t>
+    <t xml:space="preserve">Turn #2: Hello: </t>
   </si>
   <si>
     <t xml:space="preserve">Turn #3: Brobdingnag: </t>
@@ -52,7 +52,7 @@
     <t xml:space="preserve">Turn #3: Foremz: </t>
   </si>
   <si>
-    <t xml:space="preserve">Turn #3: hello: </t>
+    <t xml:space="preserve">Turn #3: Hello: </t>
   </si>
   <si>
     <t>(TRANSFORM Brobdingnag (INPUTS (Population 1) (MetallicElements 2))  (OUTPUTS (Population 1) (MetallicAlloys 1) (MetallicAlloysWaste 1))) EU: 0.2204656796309895</t>
@@ -64,25 +64,25 @@
     <t>(PASSES Foremz )</t>
   </si>
   <si>
-    <t>(TRANSFORM hello (INPUTS (Population 1) (MetallicElements 2))  (OUTPUTS (Population 1) (MetallicAlloys 1) (MetallicAlloysWaste 1))) EU: -0.09899999999999437</t>
+    <t>(TRANSFORM Hello (INPUTS (Population 5) (MetallicElements 3) (MetallicAlloys 2)) (OUTPUTS (Population 5) (Electronics 2) (ElectonicsWaste 1))) EU: 0.22096544749376973</t>
   </si>
   <si>
     <t>(TRANSFORM Brobdingnag (INPUTS (Population 1) (MetallicElements 2))  (OUTPUTS (Population 1) (MetallicAlloys 1) (MetallicAlloysWaste 1))) EU: 0.2010918779913348</t>
   </si>
   <si>
-    <t>(TRANSFORM Erewhon (INPUTS (Population 1) (MetallicElements 2))  (OUTPUTS (Population 1) (MetallicAlloys 1) (MetallicAlloysWaste 1))) EU: -0.7085605790053421</t>
-  </si>
-  <si>
-    <t>(TRANSFORM hello (INPUTS ((Population 2) (Electronics 4) (Metallic Alloys 6))(OUTPUTS (Population 2) (Electronics2) (Metallic Alloys 4) (Telecommunications 3) (TelecommunicationsWaste 1))) EU: 0.09259819278162994</t>
+    <t>(DISASTER Erewhon (Earthquake)) (TRANSFORM Erewhon (INPUTS (Population 5) (MetallicElements 3) (MetallicAlloys 2)) (OUTPUTS (Population 5) (Electronics 2) (ElectonicsWaste 1))) EU: -2.0130409724967318</t>
+  </si>
+  <si>
+    <t>(DISASTER Hello (Fire)) (TRANSFORM Hello (INPUTS (Population 1) (MetallicElements 2))  (OUTPUTS (Population 1) (MetallicAlloys 1) (MetallicAlloysWaste 1))) EU: 0.16863274528787145</t>
   </si>
   <si>
     <t>(TRANSFORM Brobdingnag (INPUTS (Population 1) (MetallicElements 2))  (OUTPUTS (Population 1) (MetallicAlloys 1) (MetallicAlloysWaste 1))) EU: 0.18393414850775172</t>
   </si>
   <si>
-    <t>(TRANSFORM Erewhon (INPUTS (Population 1) (Timber 3) (Housing 1))  (OUTPUTS (Population 1) (Food 2) (Housing 1) (FoodWaste 1))) EU: -0.2475</t>
-  </si>
-  <si>
-    <t>(TRANSFORM hello (INPUTS (Population 1) (MetallicElements 2))  (OUTPUTS (Population 1) (MetallicAlloys 1) (MetallicAlloysWaste 1))) EU: 0.15490180721837007</t>
+    <t>(DISASTER Erewhon (Tornado)) (PASSES Erewhon )</t>
+  </si>
+  <si>
+    <t>(TRANSFORM Hello (INPUTS (Population 5) (MetallicElements 3) (MetallicAlloys 2)) (OUTPUTS (Population 5) (Electronics 2) (ElectonicsWaste 1))) EU: 0.19193310620438808</t>
   </si>
 </sst>
 </file>

</xml_diff>